<commit_message>
alter table t_photo   add column moderation_result ENUM('UNCENSORED', 'OK', 'NG') comment '検閲結果' after address,   add column moderation_labels VARCHAR(128) comment '検閲詳細' after moderation_result ;
</commit_message>
<xml_diff>
--- a/src/main/resources/db/00_doc/エンティティ定義書.xlsx
+++ b/src/main/resources/db/00_doc/エンティティ定義書.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spcia\Documents\repository\cheese-sns-api\src\main\resources\db\00_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16A7E5B9-4F70-4D1D-B212-1CDE295D4090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FECFB2D8-8B97-48A5-924E-C9EEA7EF886D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{44F2FD87-0E0A-4DA0-AD56-EA80BEFF1895}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BABF510C-0DA2-4FD4-B8DA-82D80B8E81C7}"/>
   </bookViews>
   <sheets>
     <sheet name="サマリ" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="238">
   <si>
     <t>エンティティ定義書　サマリ</t>
   </si>
@@ -71,7 +71,7 @@
     <t>作成日</t>
   </si>
   <si>
-    <t>2020/04/09</t>
+    <t>2020/04/17</t>
   </si>
   <si>
     <t>エンティティ一覧</t>
@@ -621,6 +621,21 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>検閲結果</t>
+  </si>
+  <si>
+    <t>moderation_result</t>
+  </si>
+  <si>
+    <t>ENUM('UNCENSORED', 'OK', 'NG')</t>
+  </si>
+  <si>
+    <t>検閲詳細</t>
+  </si>
+  <si>
+    <t>moderation_labels</t>
   </si>
   <si>
     <t>コメントコード</t>
@@ -2118,13 +2133,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A7B551-B3B8-4375-B5E4-23270948AC93}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A517027-95F8-4E29-A8EC-EE48F55F2A3C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2648,7 +2665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B53676A-8172-4411-ABF5-0DA4615EDFDE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D123C55-BE52-428E-A145-C1E46F376DEA}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3164,7 +3181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFC5F70-EF5F-45AE-AE7A-1EB1414AF915}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2570DA6-FC76-42FD-9080-B89AF8CEC82B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3664,11 +3681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBACA00D-B5FA-4261-A903-72B22D9F7A51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91AFE88-F3E4-4E0F-B236-E9C544561514}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4084,19 +4101,17 @@
         <v>13</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>90</v>
+        <v>191</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="D26" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>62</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="E26" s="56"/>
       <c r="F26" s="65" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="G26" s="66" t="s">
         <v>48</v>
@@ -4107,19 +4122,17 @@
         <v>14</v>
       </c>
       <c r="B27" s="56" t="s">
-        <v>94</v>
+        <v>194</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>95</v>
+        <v>195</v>
       </c>
       <c r="D27" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>62</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="E27" s="56"/>
       <c r="F27" s="65" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="G27" s="66" t="s">
         <v>48</v>
@@ -4130,19 +4143,19 @@
         <v>15</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D28" s="56" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E28" s="56" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G28" s="66" t="s">
         <v>48</v>
@@ -4153,10 +4166,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D29" s="56" t="s">
         <v>96</v>
@@ -4171,197 +4184,205 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="29">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="26">
         <v>17</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="26">
+        <v>18</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="29">
+        <v>19</v>
+      </c>
+      <c r="B32" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C32" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D32" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E32" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="67" t="s">
+      <c r="F32" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="25" t="s">
+      <c r="G32" s="68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A33" s="35" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A35" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B35" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C35" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="49" t="s">
+      <c r="D35" s="70"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="G33" s="62" t="s">
+      <c r="G35" s="62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="53">
+    <row r="36" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="53">
         <v>1</v>
       </c>
-      <c r="B34" s="54" t="s">
+      <c r="B36" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C36" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="73"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="54" t="s">
+      <c r="D36" s="73"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G34" s="55"/>
-    </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="25" t="s">
+      <c r="G36" s="55"/>
+    </row>
+    <row r="38" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="25" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="35" t="s">
+    <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A39" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B39" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C39" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="90" t="s">
+      <c r="D39" s="71"/>
+      <c r="E39" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="91"/>
-      <c r="G37" s="62" t="s">
+      <c r="F39" s="91"/>
+      <c r="G39" s="62" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="53">
+    <row r="40" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="53">
         <v>1</v>
       </c>
-      <c r="B38" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="82" t="s">
+      <c r="B40" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="82" t="s">
+      <c r="D40" s="83"/>
+      <c r="E40" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="83"/>
-      <c r="G38" s="55" t="s">
+      <c r="F40" s="83"/>
+      <c r="G40" s="55" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="25" t="s">
+    <row r="42" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A41" s="35" t="s">
+    <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A43" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B43" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="69" t="s">
+      <c r="C43" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="71"/>
-      <c r="E41" s="90" t="s">
+      <c r="D43" s="71"/>
+      <c r="E43" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="91"/>
-      <c r="G41" s="62" t="s">
+      <c r="F43" s="91"/>
+      <c r="G43" s="62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A42" s="32">
+    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A44" s="32">
         <v>1</v>
       </c>
-      <c r="B42" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="88" t="s">
+      <c r="B44" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="89"/>
-      <c r="E42" s="88" t="s">
+      <c r="D44" s="89"/>
+      <c r="E44" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="89"/>
-      <c r="G42" s="61" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A43" s="26">
-        <v>2</v>
-      </c>
-      <c r="B43" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="85"/>
-      <c r="E43" s="84" t="s">
-        <v>39</v>
-      </c>
-      <c r="F43" s="85"/>
-      <c r="G43" s="57" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A44" s="26">
-        <v>3</v>
-      </c>
-      <c r="B44" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="85"/>
-      <c r="E44" s="84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="57" t="s">
+      <c r="F44" s="89"/>
+      <c r="G44" s="61" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A45" s="26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B45" s="56" t="s">
         <v>48</v>
@@ -4371,51 +4392,89 @@
       </c>
       <c r="D45" s="85"/>
       <c r="E45" s="84" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F45" s="85"/>
       <c r="G45" s="57" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="29">
+    <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A46" s="26">
+        <v>3</v>
+      </c>
+      <c r="B46" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="85"/>
+      <c r="E46" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="85"/>
+      <c r="G46" s="57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A47" s="26">
+        <v>4</v>
+      </c>
+      <c r="B47" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" s="85"/>
+      <c r="E47" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="85"/>
+      <c r="G47" s="57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="29">
         <v>5</v>
       </c>
-      <c r="B46" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="86" t="s">
+      <c r="B48" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="87"/>
-      <c r="E46" s="86" t="s">
+      <c r="D48" s="87"/>
+      <c r="E48" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F46" s="87"/>
-      <c r="G46" s="59" t="s">
+      <c r="F48" s="87"/>
+      <c r="G48" s="59" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -4438,7 +4497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4A44F1-5D80-4E9C-B40F-5D2808F12CD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D9B875-F703-4C2F-BF26-67430F25716B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4621,10 +4680,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D15" s="56" t="s">
         <v>166</v>
@@ -4852,10 +4911,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C27" s="72" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D27" s="73"/>
       <c r="E27" s="74"/>
@@ -5004,7 +5063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5CA889-DF6A-443A-95C0-C9B4C8DFE935}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5AA030-5953-4C83-BBAC-375D1C0CAB28}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5164,10 +5223,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>118</v>
@@ -5501,7 +5560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EEB244-A28D-4A37-994D-CAE2D7A8616E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62789DE-76F9-43CD-9F4B-F575D0F3B5C3}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5661,10 +5720,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>118</v>
@@ -5971,7 +6030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0090C4-A71E-400D-8173-FAA2AFFABC1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747441B5-6111-4A7A-B954-740DEE60D4F5}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6154,10 +6213,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D15" s="56" t="s">
         <v>147</v>
@@ -6429,7 +6488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFA549E-8014-409A-8928-8DD2F6999D0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D01EC2-5396-4D0D-8918-99B4E497B89F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6589,10 +6648,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>118</v>
@@ -6924,7 +6983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF382CA-9ACB-4A12-AB25-FFEC0DA2F6F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA6208A-989A-4F8B-A35D-B5088F653B8D}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7147,10 +7206,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D17" s="56" t="s">
         <v>48</v>
@@ -7168,10 +7227,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D18" s="56" t="s">
         <v>48</v>
@@ -7189,10 +7248,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D19" s="56" t="s">
         <v>48</v>
@@ -7210,10 +7269,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D20" s="56" t="s">
         <v>48</v>
@@ -7231,10 +7290,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="56" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D21" s="56" t="s">
         <v>48</v>
@@ -7252,10 +7311,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D22" s="56" t="s">
         <v>48</v>
@@ -7273,10 +7332,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D23" s="56" t="s">
         <v>48</v>
@@ -7294,10 +7353,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D24" s="56" t="s">
         <v>48</v>
@@ -7315,10 +7374,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>48</v>
@@ -7333,7 +7392,7 @@
     </row>
     <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="25" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -7341,7 +7400,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="95" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C28" s="96"/>
       <c r="D28" s="96"/>
@@ -7354,7 +7413,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="98" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C29" s="75"/>
       <c r="D29" s="75"/>
@@ -7367,7 +7426,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="81" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -7380,7 +7439,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="81" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -7393,7 +7452,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -7406,7 +7465,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="81" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -7419,7 +7478,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="81" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -7432,7 +7491,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="81" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -7445,7 +7504,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="81" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -7458,7 +7517,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="81" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -7471,7 +7530,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="81" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -7484,7 +7543,7 @@
         <v>11</v>
       </c>
       <c r="B39" s="81" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -7497,7 +7556,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="81" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -7510,7 +7569,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="81" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -7523,7 +7582,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="81" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -7536,7 +7595,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="81" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -7549,7 +7608,7 @@
         <v>16</v>
       </c>
       <c r="B44" s="81" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -7562,7 +7621,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="81" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -7575,7 +7634,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="81" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -7588,7 +7647,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="81" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -7601,7 +7660,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="81" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -7614,7 +7673,7 @@
         <v>21</v>
       </c>
       <c r="B49" s="81" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -7627,7 +7686,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="81" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -7640,7 +7699,7 @@
         <v>23</v>
       </c>
       <c r="B51" s="81" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -7784,7 +7843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD28644A-C2E8-45A8-8FF5-E145221BDA6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91CB99F-B9AD-40A2-9DF3-59C76C7E1FA5}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8020,21 +8079,21 @@
   </sheetData>
   <phoneticPr fontId="11"/>
   <hyperlinks>
-    <hyperlink ref="C3" location="'アカウント'!A1" display="'アカウント'!A1" xr:uid="{2D9DE2D7-5A56-4AB5-B273-A93C0A8B9DE1}"/>
-    <hyperlink ref="C4" location="'アクティビティ'!A1" display="'アクティビティ'!A1" xr:uid="{8F329BC9-50FF-4F28-95DD-7A52B326D2F5}"/>
-    <hyperlink ref="C5" location="'通報'!A1" display="'通報'!A1" xr:uid="{FC934D86-94ED-4E94-8DB2-804168593B77}"/>
-    <hyperlink ref="C6" location="'ブックマーク'!A1" display="'ブックマーク'!A1" xr:uid="{78C61F6B-B1B7-4F47-87ED-2CAB05E33DD4}"/>
-    <hyperlink ref="C7" location="'お問合せ'!A1" display="'お問合せ'!A1" xr:uid="{BBC516F8-741C-4A04-AA18-6965ACEF0C92}"/>
-    <hyperlink ref="C8" location="'フォロー'!A1" display="'フォロー'!A1" xr:uid="{8C3EAC29-2AA4-4BDD-ABC6-117E318526C8}"/>
-    <hyperlink ref="C9" location="'タグフォロー'!A1" display="'タグフォロー'!A1" xr:uid="{03A2C5D3-4C77-42EE-BFB8-D53075D4F02E}"/>
-    <hyperlink ref="C10" location="'ログイン履歴'!A1" display="'ログイン履歴'!A1" xr:uid="{EA01BB67-64BF-41FE-8CCC-4E95A4714EF0}"/>
-    <hyperlink ref="C11" location="'写真'!A1" display="'写真'!A1" xr:uid="{3E54D3CF-F4FA-4E6A-B7F6-379067BACD12}"/>
-    <hyperlink ref="C12" location="'写真コメント'!A1" display="'写真コメント'!A1" xr:uid="{ABEA6EFD-34AE-4872-9DDD-12A15E27787E}"/>
-    <hyperlink ref="C13" location="'写真コメントいいね'!A1" display="'写真コメントいいね'!A1" xr:uid="{C4B10728-E3FD-44A4-B692-7DD30882C2DF}"/>
-    <hyperlink ref="C14" location="'写真いいね'!A1" display="'写真いいね'!A1" xr:uid="{CE30E5D3-4AC7-4047-AF7A-122216591590}"/>
-    <hyperlink ref="C15" location="'タグ'!A1" display="'タグ'!A1" xr:uid="{2B862E4B-9A0F-4A18-B88E-5B99F51639D1}"/>
-    <hyperlink ref="C16" location="'写真タグ'!A1" display="'写真タグ'!A1" xr:uid="{63133690-E159-4DB7-860F-049CB39FC698}"/>
-    <hyperlink ref="C17" location="'フォロービュー'!A1" display="'フォロービュー'!A1" xr:uid="{AB194D07-26F4-4C3E-BF0B-1284A739C5BD}"/>
+    <hyperlink ref="C3" location="'アカウント'!A1" display="'アカウント'!A1" xr:uid="{73132F98-5106-466B-A529-90E7D66DF665}"/>
+    <hyperlink ref="C4" location="'アクティビティ'!A1" display="'アクティビティ'!A1" xr:uid="{8D80567F-FE1B-4951-B720-2B5584273F9A}"/>
+    <hyperlink ref="C5" location="'通報'!A1" display="'通報'!A1" xr:uid="{67D92951-9AA8-458E-BCD6-EC7C36BC075C}"/>
+    <hyperlink ref="C6" location="'ブックマーク'!A1" display="'ブックマーク'!A1" xr:uid="{C76B2BD2-D091-47ED-B995-E5411BF8E9BB}"/>
+    <hyperlink ref="C7" location="'お問合せ'!A1" display="'お問合せ'!A1" xr:uid="{F6B19069-4394-438D-AD48-06D80125DE3A}"/>
+    <hyperlink ref="C8" location="'フォロー'!A1" display="'フォロー'!A1" xr:uid="{5A00140F-1B1F-49E5-9091-B556376E21D8}"/>
+    <hyperlink ref="C9" location="'タグフォロー'!A1" display="'タグフォロー'!A1" xr:uid="{02478636-ECFB-49A5-A666-740B0CED1D80}"/>
+    <hyperlink ref="C10" location="'ログイン履歴'!A1" display="'ログイン履歴'!A1" xr:uid="{6BCB403B-83DC-4194-B972-739656EC7E8F}"/>
+    <hyperlink ref="C11" location="'写真'!A1" display="'写真'!A1" xr:uid="{8436FB86-0411-468B-9FED-2F2959B0D32C}"/>
+    <hyperlink ref="C12" location="'写真コメント'!A1" display="'写真コメント'!A1" xr:uid="{276061F9-5C5D-4A28-8AA1-77DBB1179CC2}"/>
+    <hyperlink ref="C13" location="'写真コメントいいね'!A1" display="'写真コメントいいね'!A1" xr:uid="{D67893E6-42FD-47AA-80C6-29014EA02197}"/>
+    <hyperlink ref="C14" location="'写真いいね'!A1" display="'写真いいね'!A1" xr:uid="{B350D400-2B17-4992-A6D6-02CADA3061E7}"/>
+    <hyperlink ref="C15" location="'タグ'!A1" display="'タグ'!A1" xr:uid="{1518C864-81E7-464F-A695-A0021E19AFD0}"/>
+    <hyperlink ref="C16" location="'写真タグ'!A1" display="'写真タグ'!A1" xr:uid="{945AE8C3-746B-4D5A-B4F9-2D14B6E8F216}"/>
+    <hyperlink ref="C17" location="'フォロービュー'!A1" display="'フォロービュー'!A1" xr:uid="{20EA7CAB-D5BE-4784-87A3-E9ED8CCD9FED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -8046,7 +8105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F42A7B-B4B3-41C2-9E2D-9E5C41CADB03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C74E757-F556-46A3-9141-00EF7CDA6CD1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8093,7 +8152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB3A701-58E9-4BEB-9ED5-F5D9676255D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8F5C92-0622-421A-AC06-31349205FBF6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8909,7 +8968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6751D8-2AD3-48A3-A539-FE0344471039}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93BE1C3-438D-45E6-A1FA-ECDF20CED1C6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9425,7 +9484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2B3021-4AF8-4718-8E51-E5B8E1D24249}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6808946F-7E43-47CA-9640-D371F49F507B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10015,7 +10074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B6E1E5-340C-46D7-AFA9-3AA7BE12BFCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA6A31C-0474-47C1-A44B-8E340931EEF4}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10487,7 +10546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BC1FDF-3E63-4CCB-962B-8E73A529665C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC6C675-49A4-4475-9E86-65FF2C5AC1ED}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10972,7 +11031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E6A954-A6E2-4117-BC2C-B5F4EE33488D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77887453-5A52-482D-912A-C636A66C33FB}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>